<commit_message>
added more error checking
</commit_message>
<xml_diff>
--- a/EXAMPLE - DocumentIndex.xlsx
+++ b/EXAMPLE - DocumentIndex.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\EPDMVault\Projects\Current\016867s L&amp;T Hydrocarbon Saudi\04 - Final Manual Books\IOM Books\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Engineering\Eli Saunders\Python\Python MRB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E3BC06C-868D-44DF-9182-425A847137E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{985411A0-05E0-47A7-950C-E390A8A75ADD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="28080" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Index" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="80">
   <si>
     <t>Project directory</t>
   </si>
@@ -177,12 +177,6 @@
     <t>Installation, Operation &amp; Maintenance Manual – Control Panel</t>
   </si>
   <si>
-    <t>Blank PDF file</t>
-  </si>
-  <si>
-    <t>Filename for the template page for table of contents and section headings.</t>
-  </si>
-  <si>
     <t>Pump Manual</t>
   </si>
   <si>
@@ -250,9 +244,6 @@
   </si>
   <si>
     <t>016867TP</t>
-  </si>
-  <si>
-    <t>TP - BlankPage.pdf</t>
   </si>
   <si>
     <t>Pump Drawings - SLPRAM-ME-G75-DW-0004</t>
@@ -1031,10 +1022,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G53"/>
+  <dimension ref="A1:G52"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1070,7 +1061,7 @@
         <v>37</v>
       </c>
       <c r="B2" s="49" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C2" s="48" t="s">
         <v>38</v>
@@ -1081,106 +1072,110 @@
       <c r="G2" s="23"/>
     </row>
     <row r="3" spans="1:7" s="8" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="B3" s="49" t="s">
-        <v>72</v>
-      </c>
-      <c r="C3" s="48" t="s">
-        <v>48</v>
+      <c r="A3" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="20">
+        <v>0</v>
+      </c>
+      <c r="C3" s="21" t="s">
+        <v>2</v>
       </c>
       <c r="D3" s="22"/>
       <c r="E3" s="29"/>
       <c r="F3" s="22"/>
       <c r="G3" s="23"/>
     </row>
-    <row r="4" spans="1:7" s="8" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B4" s="20">
-        <v>0</v>
+        <v>375</v>
       </c>
       <c r="C4" s="21" t="s">
-        <v>2</v>
-      </c>
-      <c r="D4" s="22"/>
-      <c r="E4" s="29"/>
-      <c r="F4" s="22"/>
-      <c r="G4" s="23"/>
+        <v>4</v>
+      </c>
+      <c r="D4" s="24"/>
+      <c r="E4" s="25"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="31"/>
     </row>
     <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="16" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B5" s="20">
-        <v>375</v>
-      </c>
-      <c r="C5" s="21" t="s">
-        <v>4</v>
-      </c>
-      <c r="D5" s="24"/>
-      <c r="E5" s="25"/>
-      <c r="F5" s="24"/>
-      <c r="G5" s="31"/>
-    </row>
-    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="20">
         <v>12</v>
       </c>
-      <c r="C6" s="26" t="s">
+      <c r="C5" s="26" t="s">
         <v>34</v>
       </c>
-      <c r="D6" s="27"/>
-      <c r="E6" s="30"/>
-      <c r="F6" s="27"/>
-      <c r="G6" s="32"/>
-    </row>
-    <row r="7" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="10"/>
-      <c r="B7" s="11"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="10"/>
-    </row>
-    <row r="8" spans="1:7" s="12" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="33" t="s">
+      <c r="D5" s="27"/>
+      <c r="E5" s="30"/>
+      <c r="F5" s="27"/>
+      <c r="G5" s="32"/>
+    </row>
+    <row r="6" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="10"/>
+      <c r="B6" s="11"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="10"/>
+    </row>
+    <row r="7" spans="1:7" s="12" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="13" t="s">
+      <c r="B7" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="14" t="s">
+      <c r="C7" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="13" t="s">
+      <c r="D7" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="E8" s="14" t="s">
+      <c r="E7" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="F8" s="13" t="s">
+      <c r="F7" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="G8" s="34" t="s">
+      <c r="G7" s="34" t="s">
         <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="43" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="37">
+        <v>1</v>
+      </c>
+      <c r="C8" s="41" t="s">
+        <v>41</v>
+      </c>
+      <c r="D8" s="45"/>
+      <c r="E8" s="39"/>
+      <c r="F8" s="37" t="s">
+        <v>14</v>
+      </c>
+      <c r="G8" s="35" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="43" t="s">
-        <v>13</v>
+        <v>48</v>
       </c>
       <c r="B9" s="37">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C9" s="41" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="D9" s="45"/>
       <c r="E9" s="39"/>
@@ -1193,13 +1188,13 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="43" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B10" s="37">
         <v>2</v>
       </c>
       <c r="C10" s="41" t="s">
-        <v>49</v>
+        <v>70</v>
       </c>
       <c r="D10" s="45"/>
       <c r="E10" s="39"/>
@@ -1212,13 +1207,13 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="43" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B11" s="37">
         <v>2</v>
       </c>
       <c r="C11" s="41" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D11" s="45"/>
       <c r="E11" s="39"/>
@@ -1230,35 +1225,35 @@
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="43" t="s">
-        <v>52</v>
-      </c>
-      <c r="B12" s="37">
+      <c r="A12" s="44" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="38">
+        <v>1</v>
+      </c>
+      <c r="C12" s="42" t="s">
+        <v>42</v>
+      </c>
+      <c r="D12" s="46"/>
+      <c r="F12" s="37" t="s">
+        <v>14</v>
+      </c>
+      <c r="G12" s="35" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="43" t="s">
+        <v>51</v>
+      </c>
+      <c r="B13" s="37">
         <v>2</v>
       </c>
-      <c r="C12" s="41" t="s">
-        <v>74</v>
-      </c>
-      <c r="D12" s="45"/>
-      <c r="E12" s="39"/>
-      <c r="F12" s="37" t="s">
-        <v>14</v>
-      </c>
-      <c r="G12" s="35" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="44" t="s">
-        <v>15</v>
-      </c>
-      <c r="B13" s="38">
-        <v>1</v>
-      </c>
-      <c r="C13" s="42" t="s">
-        <v>42</v>
-      </c>
-      <c r="D13" s="46"/>
+      <c r="C13" s="41" t="s">
+        <v>64</v>
+      </c>
+      <c r="D13" s="45"/>
+      <c r="E13" s="39"/>
       <c r="F13" s="37" t="s">
         <v>14</v>
       </c>
@@ -1268,13 +1263,13 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="43" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B14" s="37">
         <v>2</v>
       </c>
       <c r="C14" s="41" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="D14" s="45"/>
       <c r="E14" s="39"/>
@@ -1287,13 +1282,13 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="43" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B15" s="37">
         <v>2</v>
       </c>
       <c r="C15" s="41" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D15" s="45"/>
       <c r="E15" s="39"/>
@@ -1305,35 +1300,35 @@
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="43" t="s">
-        <v>55</v>
-      </c>
-      <c r="B16" s="37">
+      <c r="A16" s="44" t="s">
+        <v>40</v>
+      </c>
+      <c r="B16" s="38">
+        <v>1</v>
+      </c>
+      <c r="C16" s="42" t="s">
+        <v>43</v>
+      </c>
+      <c r="D16" s="46"/>
+      <c r="F16" s="37" t="s">
+        <v>14</v>
+      </c>
+      <c r="G16" s="35" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="43" t="s">
+        <v>54</v>
+      </c>
+      <c r="B17" s="37">
         <v>2</v>
       </c>
-      <c r="C16" s="41" t="s">
-        <v>76</v>
-      </c>
-      <c r="D16" s="45"/>
-      <c r="E16" s="39"/>
-      <c r="F16" s="37" t="s">
-        <v>14</v>
-      </c>
-      <c r="G16" s="35" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="B17" s="38">
-        <v>1</v>
-      </c>
-      <c r="C17" s="42" t="s">
-        <v>43</v>
-      </c>
-      <c r="D17" s="46"/>
+      <c r="C17" s="41" t="s">
+        <v>63</v>
+      </c>
+      <c r="D17" s="45"/>
+      <c r="E17" s="39"/>
       <c r="F17" s="37" t="s">
         <v>14</v>
       </c>
@@ -1343,13 +1338,13 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="43" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B18" s="37">
         <v>2</v>
       </c>
       <c r="C18" s="41" t="s">
-        <v>65</v>
+        <v>74</v>
       </c>
       <c r="D18" s="45"/>
       <c r="E18" s="39"/>
@@ -1362,13 +1357,13 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="43" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B19" s="37">
         <v>2</v>
       </c>
       <c r="C19" s="41" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D19" s="45"/>
       <c r="E19" s="39"/>
@@ -1381,16 +1376,15 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="43" t="s">
-        <v>58</v>
+        <v>16</v>
       </c>
       <c r="B20" s="37">
-        <v>2</v>
-      </c>
-      <c r="C20" s="41" t="s">
-        <v>78</v>
-      </c>
-      <c r="D20" s="45"/>
-      <c r="E20" s="39"/>
+        <v>1</v>
+      </c>
+      <c r="C20" s="42" t="s">
+        <v>44</v>
+      </c>
+      <c r="D20" s="46"/>
       <c r="F20" s="37" t="s">
         <v>14</v>
       </c>
@@ -1400,15 +1394,16 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="43" t="s">
-        <v>16</v>
+        <v>57</v>
       </c>
       <c r="B21" s="37">
-        <v>1</v>
-      </c>
-      <c r="C21" s="42" t="s">
-        <v>44</v>
-      </c>
-      <c r="D21" s="46"/>
+        <v>2</v>
+      </c>
+      <c r="C21" s="41" t="s">
+        <v>65</v>
+      </c>
+      <c r="D21" s="45"/>
+      <c r="E21" s="39"/>
       <c r="F21" s="37" t="s">
         <v>14</v>
       </c>
@@ -1418,13 +1413,13 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="43" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B22" s="37">
         <v>2</v>
       </c>
       <c r="C22" s="41" t="s">
-        <v>67</v>
+        <v>76</v>
       </c>
       <c r="D22" s="45"/>
       <c r="E22" s="39"/>
@@ -1436,35 +1431,35 @@
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="43" t="s">
-        <v>60</v>
-      </c>
-      <c r="B23" s="37">
+      <c r="A23" s="44" t="s">
+        <v>17</v>
+      </c>
+      <c r="B23" s="38">
+        <v>1</v>
+      </c>
+      <c r="C23" s="42" t="s">
+        <v>45</v>
+      </c>
+      <c r="D23" s="46"/>
+      <c r="F23" s="37" t="s">
+        <v>14</v>
+      </c>
+      <c r="G23" s="35" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="43" t="s">
+        <v>59</v>
+      </c>
+      <c r="B24" s="37">
         <v>2</v>
       </c>
-      <c r="C23" s="41" t="s">
-        <v>79</v>
-      </c>
-      <c r="D23" s="45"/>
-      <c r="E23" s="39"/>
-      <c r="F23" s="37" t="s">
-        <v>14</v>
-      </c>
-      <c r="G23" s="35" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="44" t="s">
-        <v>17</v>
-      </c>
-      <c r="B24" s="38">
-        <v>1</v>
-      </c>
-      <c r="C24" s="42" t="s">
-        <v>45</v>
-      </c>
-      <c r="D24" s="46"/>
+      <c r="C24" s="41" t="s">
+        <v>66</v>
+      </c>
+      <c r="D24" s="45"/>
+      <c r="E24" s="39"/>
       <c r="F24" s="37" t="s">
         <v>14</v>
       </c>
@@ -1474,13 +1469,13 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="43" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B25" s="37">
         <v>2</v>
       </c>
       <c r="C25" s="41" t="s">
-        <v>68</v>
+        <v>77</v>
       </c>
       <c r="D25" s="45"/>
       <c r="E25" s="39"/>
@@ -1493,13 +1488,13 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="43" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="B26" s="37">
         <v>2</v>
       </c>
       <c r="C26" s="41" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D26" s="45"/>
       <c r="E26" s="39"/>
@@ -1511,35 +1506,35 @@
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="43" t="s">
-        <v>70</v>
-      </c>
-      <c r="B27" s="37">
+      <c r="A27" s="44" t="s">
+        <v>18</v>
+      </c>
+      <c r="B27" s="38">
+        <v>1</v>
+      </c>
+      <c r="C27" s="42" t="s">
+        <v>46</v>
+      </c>
+      <c r="D27" s="47"/>
+      <c r="F27" s="37" t="s">
+        <v>14</v>
+      </c>
+      <c r="G27" s="35" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="43" t="s">
+        <v>61</v>
+      </c>
+      <c r="B28" s="37">
         <v>2</v>
       </c>
-      <c r="C27" s="41" t="s">
-        <v>81</v>
-      </c>
-      <c r="D27" s="45"/>
-      <c r="E27" s="39"/>
-      <c r="F27" s="37" t="s">
-        <v>14</v>
-      </c>
-      <c r="G27" s="35" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="44" t="s">
-        <v>18</v>
-      </c>
-      <c r="B28" s="38">
-        <v>1</v>
-      </c>
-      <c r="C28" s="42" t="s">
-        <v>46</v>
-      </c>
-      <c r="D28" s="47"/>
+      <c r="C28" s="41" t="s">
+        <v>67</v>
+      </c>
+      <c r="D28" s="45"/>
+      <c r="E28" s="39"/>
       <c r="F28" s="37" t="s">
         <v>14</v>
       </c>
@@ -1549,13 +1544,13 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="43" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B29" s="37">
         <v>2</v>
       </c>
       <c r="C29" s="41" t="s">
-        <v>69</v>
+        <v>79</v>
       </c>
       <c r="D29" s="45"/>
       <c r="E29" s="39"/>
@@ -1567,35 +1562,20 @@
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="43" t="s">
-        <v>64</v>
-      </c>
-      <c r="B30" s="37">
-        <v>2</v>
-      </c>
-      <c r="C30" s="41" t="s">
-        <v>82</v>
-      </c>
-      <c r="D30" s="45"/>
-      <c r="E30" s="39"/>
-      <c r="F30" s="37" t="s">
-        <v>14</v>
-      </c>
-      <c r="G30" s="35" t="s">
-        <v>14</v>
-      </c>
+      <c r="C30" s="42"/>
+      <c r="D30" s="46"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C31" s="42"/>
-      <c r="D31" s="46"/>
+      <c r="D31" s="47"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="43"/>
+      <c r="B32" s="37"/>
       <c r="C32" s="42"/>
-      <c r="D32" s="47"/>
+      <c r="D32" s="46"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="43"/>
-      <c r="B33" s="37"/>
       <c r="C33" s="42"/>
       <c r="D33" s="46"/>
     </row>
@@ -1604,12 +1584,12 @@
       <c r="D34" s="46"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="43"/>
+      <c r="B35" s="37"/>
       <c r="C35" s="42"/>
       <c r="D35" s="46"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="43"/>
-      <c r="B36" s="37"/>
       <c r="C36" s="42"/>
       <c r="D36" s="46"/>
     </row>
@@ -1618,12 +1598,12 @@
       <c r="D37" s="46"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="43"/>
+      <c r="B38" s="37"/>
       <c r="C38" s="42"/>
       <c r="D38" s="46"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="43"/>
-      <c r="B39" s="37"/>
       <c r="C39" s="42"/>
       <c r="D39" s="46"/>
     </row>
@@ -1632,12 +1612,12 @@
       <c r="D40" s="46"/>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="43"/>
+      <c r="B41" s="37"/>
       <c r="C41" s="42"/>
       <c r="D41" s="46"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="43"/>
-      <c r="B42" s="37"/>
       <c r="C42" s="42"/>
       <c r="D42" s="46"/>
     </row>
@@ -1646,22 +1626,22 @@
       <c r="D43" s="46"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="43"/>
+      <c r="B44" s="37"/>
       <c r="C44" s="42"/>
       <c r="D44" s="46"/>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="43"/>
-      <c r="B45" s="37"/>
       <c r="C45" s="42"/>
       <c r="D45" s="46"/>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="43"/>
+      <c r="B46" s="37"/>
       <c r="C46" s="42"/>
       <c r="D46" s="46"/>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="43"/>
-      <c r="B47" s="37"/>
       <c r="C47" s="42"/>
       <c r="D47" s="46"/>
     </row>
@@ -1670,12 +1650,12 @@
       <c r="D48" s="46"/>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="43"/>
+      <c r="B49" s="37"/>
       <c r="C49" s="42"/>
       <c r="D49" s="46"/>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="43"/>
-      <c r="B50" s="37"/>
       <c r="C50" s="42"/>
       <c r="D50" s="46"/>
     </row>
@@ -1687,31 +1667,27 @@
       <c r="C52" s="42"/>
       <c r="D52" s="46"/>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C53" s="42"/>
-      <c r="D53" s="46"/>
-    </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
-  <conditionalFormatting sqref="E31:E1048576 E28 E24 E8:E13 F1:F7 E17 E21">
+  <conditionalFormatting sqref="E30:E1048576 E27 E23 E7:E12 F1:F6 E16 E20">
     <cfRule type="duplicateValues" dxfId="6" priority="7"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E14:E16">
+  <conditionalFormatting sqref="E13:E15">
     <cfRule type="duplicateValues" dxfId="5" priority="6"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E18:E20">
+  <conditionalFormatting sqref="E17:E19">
     <cfRule type="duplicateValues" dxfId="4" priority="5"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E25:E26">
+  <conditionalFormatting sqref="E24:E25">
     <cfRule type="duplicateValues" dxfId="3" priority="14"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E29:E30">
+  <conditionalFormatting sqref="E28:E29">
     <cfRule type="duplicateValues" dxfId="2" priority="21"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E22:E23">
+  <conditionalFormatting sqref="E21:E22">
     <cfRule type="duplicateValues" dxfId="1" priority="28"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E27">
+  <conditionalFormatting sqref="E26">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>